<commit_message>
add job titles validations
</commit_message>
<xml_diff>
--- a/data/OrangeHRMS.xlsx
+++ b/data/OrangeHRMS.xlsx
@@ -9,14 +9,13 @@
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Data" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
   <si>
     <t>Test_Case_Name</t>
   </si>
@@ -132,9 +131,6 @@
     <t>Design software systems</t>
   </si>
   <si>
-    <t>Write code to make solve a business problem</t>
-  </si>
-  <si>
     <t>JobTitleTest</t>
   </si>
   <si>
@@ -148,6 +144,15 @@
   </si>
   <si>
     <t>Write test cases</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Write code to solve a business problem</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
   </si>
 </sst>
 </file>
@@ -564,12 +569,12 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>10</v>
@@ -589,10 +594,10 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -763,7 +768,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -777,12 +782,15 @@
         <v>34</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>35</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -798,9 +806,12 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -809,16 +820,19 @@
         <v>7</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="G16" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -826,16 +840,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added delete job titles test
</commit_message>
<xml_diff>
--- a/data/OrangeHRMS.xlsx
+++ b/data/OrangeHRMS.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="53">
   <si>
     <t>Test_Case_Name</t>
   </si>
@@ -153,6 +153,27 @@
   </si>
   <si>
     <t>Duplicate</t>
+  </si>
+  <si>
+    <t>DeleteJobTitleTest</t>
+  </si>
+  <si>
+    <t>Test Architect</t>
+  </si>
+  <si>
+    <t>Design automation frameworks</t>
+  </si>
+  <si>
+    <t>Write code to automate testing</t>
+  </si>
+  <si>
+    <t>DeleteTitleTest</t>
+  </si>
+  <si>
+    <t>Network Engineer</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
   </si>
 </sst>
 </file>
@@ -547,13 +568,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -577,6 +598,14 @@
         <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -587,9 +616,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -836,6 +867,88 @@
         <v>10</v>
       </c>
     </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added edit job title test
</commit_message>
<xml_diff>
--- a/data/OrangeHRMS.xlsx
+++ b/data/OrangeHRMS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="42">
   <si>
     <t>Test_Case_Name</t>
   </si>
@@ -50,66 +50,12 @@
     <t>Y</t>
   </si>
   <si>
-    <t>BrowerName</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Pincode</t>
-  </si>
-  <si>
     <t>xyzsa</t>
   </si>
   <si>
     <t>Fail</t>
   </si>
   <si>
-    <t>Frank</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>Boriavli</t>
-  </si>
-  <si>
-    <t>AddEmployeeTest</t>
-  </si>
-  <si>
-    <t>Sunil</t>
-  </si>
-  <si>
-    <t>Pal</t>
-  </si>
-  <si>
-    <t>Malad</t>
-  </si>
-  <si>
-    <t>Rajpal</t>
-  </si>
-  <si>
-    <t>Yadav</t>
-  </si>
-  <si>
-    <t>Andheri</t>
-  </si>
-  <si>
-    <t>400103</t>
-  </si>
-  <si>
-    <t>400078</t>
-  </si>
-  <si>
-    <t>400054</t>
-  </si>
-  <si>
     <t>jack</t>
   </si>
   <si>
@@ -174,6 +120,27 @@
   </si>
   <si>
     <t>Project Manager</t>
+  </si>
+  <si>
+    <t>EditTitleTest</t>
+  </si>
+  <si>
+    <t>Old Job Title</t>
+  </si>
+  <si>
+    <t>New Job Title</t>
+  </si>
+  <si>
+    <t>Business Analyst</t>
+  </si>
+  <si>
+    <t>ICT Business Analyst</t>
+  </si>
+  <si>
+    <t>Network Security Engineer</t>
+  </si>
+  <si>
+    <t>EditJobTitleTest</t>
   </si>
 </sst>
 </file>
@@ -257,15 +224,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -568,9 +532,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -590,12 +556,12 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>10</v>
@@ -603,9 +569,17 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -616,11 +590,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -631,12 +603,12 @@
     <col min="5" max="5" width="42.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -653,7 +625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -670,7 +642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -678,274 +650,271 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="F8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="F11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="C17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="2" t="s">
+      <c r="C23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding code to handle job specification upload
</commit_message>
<xml_diff>
--- a/data/OrangeHRMS.xlsx
+++ b/data/OrangeHRMS.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="56">
   <si>
     <t>Test_Case_Name</t>
   </si>
@@ -141,6 +141,48 @@
   </si>
   <si>
     <t>EditJobTitleTest</t>
+  </si>
+  <si>
+    <t>Manage and setup the network</t>
+  </si>
+  <si>
+    <t>Maintain and add new components to the network</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>Keep Current</t>
+  </si>
+  <si>
+    <t>E:\Selenium\OrangeHRM\OrangeHRMS_DDF_Framework\abc.xml</t>
+  </si>
+  <si>
+    <t>Sr. Software Tester</t>
+  </si>
+  <si>
+    <t>QA Engineer</t>
+  </si>
+  <si>
+    <t>Find faults and defects in the software quality process</t>
+  </si>
+  <si>
+    <t>Write and maintain the quality assurance process</t>
+  </si>
+  <si>
+    <t>Delete Current</t>
+  </si>
+  <si>
+    <t>Replace Current</t>
+  </si>
+  <si>
+    <t>Attachment</t>
+  </si>
+  <si>
+    <t>E:\Selenium\OrangeHRM\OrangeHRMS_DDF_Framework\extentreports\abc.xml</t>
+  </si>
+  <si>
+    <t>Sr. Software Engineer</t>
   </si>
 </sst>
 </file>
@@ -590,7 +632,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -599,8 +641,8 @@
     <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -714,7 +756,9 @@
       <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="E9" s="2" t="s">
         <v>26</v>
       </c>
@@ -735,7 +779,9 @@
       <c r="C10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="E10" s="4" t="s">
         <v>24</v>
       </c>
@@ -767,154 +813,327 @@
         <v>10</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="2" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="D20" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="D21" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="2" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="2" t="s">
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="2" t="s">
+      <c r="G26" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="4" t="s">
+      <c r="G27" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C28" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="C29" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="G29" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="4" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding code to check success msg
</commit_message>
<xml_diff>
--- a/data/OrangeHRMS.xlsx
+++ b/data/OrangeHRMS.xlsx
@@ -577,7 +577,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +614,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -622,7 +622,7 @@
         <v>41</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -634,7 +634,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -766,7 +768,7 @@
         <v>10</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -789,7 +791,7 @@
         <v>25</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -810,7 +812,7 @@
         <v>25</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -829,7 +831,7 @@
         <v>25</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -852,7 +854,7 @@
         <v>10</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -875,7 +877,7 @@
         <v>25</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -945,7 +947,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -959,7 +961,7 @@
         <v>12</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added code to read notication message
</commit_message>
<xml_diff>
--- a/data/OrangeHRMS.xlsx
+++ b/data/OrangeHRMS.xlsx
@@ -576,9 +576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -614,7 +612,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -622,7 +620,7 @@
         <v>41</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -634,9 +632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -768,7 +764,7 @@
         <v>10</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -791,7 +787,7 @@
         <v>25</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -812,7 +808,7 @@
         <v>25</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -831,7 +827,7 @@
         <v>25</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -854,7 +850,7 @@
         <v>10</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -877,7 +873,7 @@
         <v>25</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -947,7 +943,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -961,7 +957,7 @@
         <v>12</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1016,10 +1012,10 @@
         <v>7</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2" t="s">

</xml_diff>

<commit_message>
added code to pay grades
</commit_message>
<xml_diff>
--- a/data/OrangeHRMS.xlsx
+++ b/data/OrangeHRMS.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="75">
   <si>
     <t>Test_Case_Name</t>
   </si>
@@ -206,10 +206,40 @@
     <t>100000</t>
   </si>
   <si>
-    <t>ten thousand</t>
-  </si>
-  <si>
     <t>Class 3</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>Class 4</t>
+  </si>
+  <si>
+    <t>AUD</t>
+  </si>
+  <si>
+    <t>Grade A</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>250000</t>
+  </si>
+  <si>
+    <t>350000</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>2500000</t>
+  </si>
+  <si>
+    <t>Grade B</t>
+  </si>
+  <si>
+    <t>Grade C</t>
   </si>
 </sst>
 </file>
@@ -668,7 +698,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1173,12 +1203,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
@@ -1195,26 +1225,139 @@
         <v>60</v>
       </c>
       <c r="F34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>62</v>
       </c>
       <c r="F35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added code to paygrades
</commit_message>
<xml_diff>
--- a/data/OrangeHRMS.xlsx
+++ b/data/OrangeHRMS.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="80">
   <si>
     <t>Test_Case_Name</t>
   </si>
@@ -240,6 +240,21 @@
   </si>
   <si>
     <t>Grade C</t>
+  </si>
+  <si>
+    <t>LKR</t>
+  </si>
+  <si>
+    <t>five lakhs</t>
+  </si>
+  <si>
+    <t>NZD</t>
+  </si>
+  <si>
+    <t>350000.25</t>
+  </si>
+  <si>
+    <t>325625</t>
   </si>
 </sst>
 </file>
@@ -705,7 +720,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="34.7109375" customWidth="1"/>
@@ -1251,7 +1266,7 @@
         <v>10</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1274,7 +1289,7 @@
         <v>25</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1308,10 +1323,10 @@
         <v>73</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>72</v>
@@ -1320,7 +1335,7 @@
         <v>25</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1341,7 +1356,7 @@
         <v>25</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1351,9 +1366,15 @@
       <c r="B40" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
+      <c r="C40" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="F40" s="2" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
delete pay grades added
</commit_message>
<xml_diff>
--- a/data/OrangeHRMS.xlsx
+++ b/data/OrangeHRMS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="82">
   <si>
     <t>Test_Case_Name</t>
   </si>
@@ -255,6 +255,12 @@
   </si>
   <si>
     <t>325625</t>
+  </si>
+  <si>
+    <t>DeletePayGradesTest</t>
+  </si>
+  <si>
+    <t>Grade E</t>
   </si>
 </sst>
 </file>
@@ -647,15 +653,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -703,6 +709,14 @@
         <v>56</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -713,14 +727,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="34.7109375" customWidth="1"/>
@@ -1303,7 +1316,7 @@
         <v>66</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>69</v>
@@ -1326,7 +1339,7 @@
         <v>77</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>72</v>
@@ -1379,6 +1392,53 @@
         <v>25</v>
       </c>
       <c r="G40" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>